<commit_message>
calculating number per genotype
</commit_message>
<xml_diff>
--- a/data/renataMilho21062022.xlsx
+++ b/data/renataMilho21062022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1126006\OneDrive - Syngenta\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syngenta-my.sharepoint.com/personal/chris_simoes_syngenta_com/Documents/Documents/AnalysisR/reporteSemanal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{B2A989E6-37EE-4B59-B261-C2B3B3FF31E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5E83C41-CC66-40FE-A3C6-E6BE188CB08A}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{B2A989E6-37EE-4B59-B261-C2B3B3FF31E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF168621-60DA-4198-B4F6-3687C5FF8264}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{8FEB7CC0-DEBA-42E6-AD3D-8535F126D1BB}"/>
+    <workbookView xWindow="31905" yWindow="1845" windowWidth="21600" windowHeight="13635" xr2:uid="{8FEB7CC0-DEBA-42E6-AD3D-8535F126D1BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Checks" sheetId="1" r:id="rId1"/>
@@ -304,7 +304,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +340,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -373,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -405,6 +413,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +432,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -719,21 +728,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29D389B-97BC-42FC-B053-6B8F9EDC5893}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -763,14 +771,14 @@
       </c>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1">
@@ -792,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -821,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -850,7 +858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -879,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -908,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -937,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -966,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -995,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>21</v>
       </c>
@@ -1024,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
@@ -1053,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -1082,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
@@ -1111,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1140,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
@@ -1169,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>28</v>
       </c>
@@ -1198,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>29</v>
       </c>
@@ -1227,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>30</v>
       </c>
@@ -1256,7 +1264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1285,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>9</v>
       </c>
@@ -1314,7 +1322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1343,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>33</v>
       </c>
@@ -1372,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>19</v>
       </c>
@@ -1401,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>34</v>
       </c>
@@ -1430,7 +1438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1459,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1488,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1517,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1546,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1575,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1604,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>29</v>
       </c>
@@ -1633,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -1662,7 +1670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1691,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1720,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1749,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1778,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -1807,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1836,7 +1844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1865,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1894,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1923,7 +1931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1952,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -1981,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2010,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -2039,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -2068,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>24</v>
       </c>
@@ -2097,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -2126,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>38</v>
       </c>
@@ -2155,7 +2163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -2184,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -2213,7 +2221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>45</v>
       </c>
@@ -2242,7 +2250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -2271,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -2300,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>40</v>
       </c>
@@ -2329,7 +2337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -2358,7 +2366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>24</v>
       </c>
@@ -2387,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -2418,11 +2426,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I58" xr:uid="{E555BD61-AA47-4F5E-8016-6E282C4ABF78}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="COSTR"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I58">
       <sortCondition ref="C2"/>
     </sortState>
@@ -2441,13 +2444,13 @@
       <selection activeCell="B15" sqref="A2:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -2455,7 +2458,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2463,7 +2466,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -2471,7 +2474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -2479,7 +2482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -2487,7 +2490,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -2495,7 +2498,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -2503,7 +2506,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -2511,7 +2514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -2519,7 +2522,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -2527,7 +2530,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -2535,7 +2538,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -2551,7 +2554,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -2559,7 +2562,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -2585,6 +2588,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D703901F2448C4468556EC33555FD21E" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1b092bb036adc0ee03e34c9fb9d5ed2b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b0f4d082-33bf-465b-a471-582773e71549" xmlns:ns4="b2b53afc-9144-4bc3-bc8b-13c82b22d0b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1dd4e391ffdfdd8c1bc616fe32eee5e9" ns3:_="" ns4:_="">
     <xsd:import namespace="b0f4d082-33bf-465b-a471-582773e71549"/>
@@ -2781,20 +2790,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AE38266-2CD4-4521-A9E3-C5C5D044A263}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AE38266-2CD4-4521-A9E3-C5C5D044A263}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DDAB3BA-49BD-4FDE-9183-54FB73D0563F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3C695BA-6581-4BF7-AE76-E95F87806E4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3C695BA-6581-4BF7-AE76-E95F87806E4C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DDAB3BA-49BD-4FDE-9183-54FB73D0563F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b0f4d082-33bf-465b-a471-582773e71549"/>
+    <ds:schemaRef ds:uri="b2b53afc-9144-4bc3-bc8b-13c82b22d0b4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>